<commit_message>
most switches & leds ready
</commit_message>
<xml_diff>
--- a/board Overviews.xlsx
+++ b/board Overviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a50f0f76735a0c6b/Documents/Pinball/PortalPinball-V4.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="549" documentId="8_{71A0D3BC-EF29-42BB-95C3-409B160B156F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02AE4BBA-F52A-4D4D-BC75-A03086E45A88}"/>
+  <xr:revisionPtr revIDLastSave="595" documentId="8_{71A0D3BC-EF29-42BB-95C3-409B160B156F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8F4BEE1-127C-4B4A-850F-3E1D7596E42D}"/>
   <bookViews>
     <workbookView xWindow="4920" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="725" xr2:uid="{992D9940-FEE0-4AED-9001-DC6BE0040B0B}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="397">
   <si>
     <t>PSOC4200</t>
   </si>
@@ -608,15 +608,6 @@
     <t>s_bottomlane5 - not on field</t>
   </si>
   <si>
-    <t>s_Other03</t>
-  </si>
-  <si>
-    <t>s_Other04</t>
-  </si>
-  <si>
-    <t>s_Other05</t>
-  </si>
-  <si>
     <t>s_drop1</t>
   </si>
   <si>
@@ -632,18 +623,6 @@
     <t>s_vukmid</t>
   </si>
   <si>
-    <t>s_Other06</t>
-  </si>
-  <si>
-    <t>s_Other07</t>
-  </si>
-  <si>
-    <t>s_Other08</t>
-  </si>
-  <si>
-    <t>s_Other09</t>
-  </si>
-  <si>
     <t>c_drop</t>
   </si>
   <si>
@@ -1118,9 +1097,6 @@
     <t>right ramp</t>
   </si>
   <si>
-    <t>missing switches</t>
-  </si>
-  <si>
     <t>led-launch</t>
   </si>
   <si>
@@ -1278,6 +1254,54 @@
   </si>
   <si>
     <t>0-0-49</t>
+  </si>
+  <si>
+    <t>s-ramp-r1</t>
+  </si>
+  <si>
+    <t>s-ramp-l1</t>
+  </si>
+  <si>
+    <t>s-ramp-r2</t>
+  </si>
+  <si>
+    <t>s-ramp-l2</t>
+  </si>
+  <si>
+    <t>s-target-e1</t>
+  </si>
+  <si>
+    <t>s-target-e2</t>
+  </si>
+  <si>
+    <t>s-button</t>
+  </si>
+  <si>
+    <t>s-orbit-top</t>
+  </si>
+  <si>
+    <t>&lt;shot&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ball drain&gt;</t>
+  </si>
+  <si>
+    <t>s-portal-r</t>
+  </si>
+  <si>
+    <t>s-dropper</t>
+  </si>
+  <si>
+    <t>s-aerial</t>
+  </si>
+  <si>
+    <t>s-insinerator</t>
+  </si>
+  <si>
+    <t>s-exit-success</t>
+  </si>
+  <si>
+    <t>s-portal-m</t>
   </si>
 </sst>
 </file>
@@ -1617,6 +1641,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1634,15 +1667,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2275,10 +2299,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2576,10 +2596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504015E5-CEAB-419C-A33C-D2331DC4ED29}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30:N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2599,51 +2619,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K1" t="s">
         <v>266</v>
-      </c>
-      <c r="E1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="G1" t="s">
-        <v>266</v>
-      </c>
-      <c r="H1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I1" t="s">
-        <v>269</v>
-      </c>
-      <c r="J1" t="s">
-        <v>326</v>
-      </c>
-      <c r="K1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E2" t="s">
         <v>157</v>
@@ -2652,19 +2672,19 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="I2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="K2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -2672,7 +2692,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E3" t="s">
         <v>158</v>
@@ -2681,16 +2701,16 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="I3" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J3" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -2698,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E4" t="s">
         <v>159</v>
@@ -2707,36 +2727,36 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H4" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="I4" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="J4" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E6" t="s">
         <v>160</v>
       </c>
       <c r="I6" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="K6" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -2744,13 +2764,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E7" t="s">
         <v>161</v>
       </c>
       <c r="I7" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -2758,13 +2778,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E8" t="s">
         <v>162</v>
       </c>
       <c r="I8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
@@ -2772,30 +2792,30 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E9" t="s">
         <v>163</v>
       </c>
       <c r="I9" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E11" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="I11" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
@@ -2803,18 +2823,18 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I12" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -2823,27 +2843,27 @@
         <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F14" s="1">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H14" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="I14" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="J14" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -2852,165 +2872,165 @@
         <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="H16" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I16" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="J16" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E18" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="I18" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="K18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E19" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="I19" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E20" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="I20" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E21" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="I21" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E22" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="I22" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E23" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I23" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E25" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="I25" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="K25" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E26" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="I26" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E27" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I27" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -3018,21 +3038,31 @@
       <c r="D29" t="s">
         <v>148</v>
       </c>
-      <c r="E29" s="32"/>
+      <c r="E29" s="47" t="s">
+        <v>381</v>
+      </c>
       <c r="F29" s="1">
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>292</v>
-      </c>
-      <c r="H29" s="32"/>
+        <v>285</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>383</v>
+      </c>
       <c r="I29" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="47"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -3040,304 +3070,344 @@
       <c r="D31" t="s">
         <v>148</v>
       </c>
-      <c r="E31" s="32"/>
+      <c r="E31" s="47" t="s">
+        <v>382</v>
+      </c>
       <c r="F31" s="1">
         <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>292</v>
-      </c>
-      <c r="H31" s="32"/>
+        <v>285</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>384</v>
+      </c>
       <c r="I31" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>268</v>
-      </c>
-      <c r="E33" s="32"/>
+        <v>261</v>
+      </c>
+      <c r="E33" s="47" t="s">
+        <v>385</v>
+      </c>
       <c r="I33" t="s">
-        <v>347</v>
-      </c>
-      <c r="M33" s="32" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>268</v>
-      </c>
-      <c r="E34" s="32"/>
+        <v>261</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>386</v>
+      </c>
       <c r="I34" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C36" s="1">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>342</v>
-      </c>
-      <c r="E36" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>387</v>
+      </c>
       <c r="I36" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E37" s="42"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="C38" s="1">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E38" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I38" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="J38" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="K38" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E39" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I39" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="J39" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E40" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I40" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="J40" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E41" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I41" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="J41" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E42" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I42" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="J42" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>268</v>
-      </c>
-      <c r="E44" s="42" t="s">
-        <v>316</v>
+        <v>261</v>
+      </c>
+      <c r="E44" t="s">
+        <v>309</v>
       </c>
       <c r="I44" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="B47" t="s">
-        <v>298</v>
-      </c>
-      <c r="E47" s="32"/>
+        <v>291</v>
+      </c>
+      <c r="E47" s="47" t="s">
+        <v>388</v>
+      </c>
       <c r="I47" s="23" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E48" s="47"/>
       <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>299</v>
-      </c>
-      <c r="E49" s="32"/>
+        <v>292</v>
+      </c>
+      <c r="E49" s="47" t="s">
+        <v>389</v>
+      </c>
       <c r="I49" s="23" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E50" s="47"/>
       <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B51" t="s">
-        <v>289</v>
-      </c>
-      <c r="E51" s="32"/>
+        <v>282</v>
+      </c>
+      <c r="E51" s="47" t="s">
+        <v>390</v>
+      </c>
       <c r="I51" s="23" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B55" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C55" s="1">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>342</v>
-      </c>
-      <c r="E55" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E55" s="47" t="s">
+        <v>391</v>
+      </c>
       <c r="I55" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="C56" s="1">
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>342</v>
-      </c>
-      <c r="E56" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E56" s="47" t="s">
+        <v>392</v>
+      </c>
       <c r="I56" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="C57" s="1">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>342</v>
-      </c>
-      <c r="E57" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E57" s="47" t="s">
+        <v>395</v>
+      </c>
       <c r="I57" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>342</v>
-      </c>
-      <c r="E58" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E58" s="47" t="s">
+        <v>393</v>
+      </c>
       <c r="I58" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
       </c>
       <c r="D59" t="s">
+        <v>334</v>
+      </c>
+      <c r="E59" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="I59" t="s">
         <v>342</v>
-      </c>
-      <c r="E59" s="32"/>
-      <c r="I59" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C60" s="1">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>342</v>
-      </c>
-      <c r="E60" s="32"/>
+        <v>334</v>
+      </c>
+      <c r="E60" s="47" t="s">
+        <v>394</v>
+      </c>
       <c r="I60" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3357,36 +3427,36 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="18" spans="2:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3443,29 +3513,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="D1" s="46" t="s">
+      <c r="B1" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="45" t="s">
-        <v>190</v>
-      </c>
       <c r="G1" s="32" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>317</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>319</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>318</v>
+        <v>310</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
@@ -3476,11 +3546,11 @@
       <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="40" t="s">
         <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
@@ -3489,13 +3559,13 @@
         <v>led-save</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D3" s="47" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
@@ -3504,13 +3574,13 @@
         <v>led-lane-b1</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D4" s="47" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="40" t="s">
         <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
@@ -3519,13 +3589,13 @@
         <v>led-lane-b2</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D5" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
@@ -3534,13 +3604,13 @@
         <v>led-sling-r</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D6" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
@@ -3549,13 +3619,13 @@
         <v>led-sling-l</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="47" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
@@ -3564,13 +3634,13 @@
         <v>led-lane-b3</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="40" t="s">
         <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
@@ -3579,13 +3649,13 @@
         <v>led-lane-b4</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
-      </c>
-      <c r="D9" s="47" t="s">
+        <v>208</v>
+      </c>
+      <c r="D9" s="40" t="s">
         <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
@@ -3594,13 +3664,13 @@
         <v>led-target-r1</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="47" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="40" t="s">
         <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
@@ -3609,13 +3679,13 @@
         <v>led-target-r2</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
-      </c>
-      <c r="D11" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="40" t="s">
         <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.35">
@@ -3624,13 +3694,13 @@
         <v>led-orbit-r</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="D12" s="40" t="s">
         <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
@@ -3639,13 +3709,13 @@
         <v>led-ramp-r</v>
       </c>
       <c r="C13" t="s">
-        <v>225</v>
-      </c>
-      <c r="D13" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="D13" s="40" t="s">
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
@@ -3654,13 +3724,13 @@
         <v>led-target-m1</v>
       </c>
       <c r="C14" t="s">
-        <v>259</v>
-      </c>
-      <c r="D14" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="D14" s="40" t="s">
         <v>107</v>
       </c>
       <c r="E14" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
@@ -3669,13 +3739,13 @@
         <v>led-portal-r</v>
       </c>
       <c r="C15" t="s">
-        <v>227</v>
-      </c>
-      <c r="D15" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="D15" s="40" t="s">
         <v>108</v>
       </c>
       <c r="E15" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
@@ -3684,13 +3754,13 @@
         <v>led-target-m2</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
-      </c>
-      <c r="D16" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="40" t="s">
         <v>109</v>
       </c>
       <c r="E16" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
@@ -3699,13 +3769,13 @@
         <v>led-bumper-1</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
-      </c>
-      <c r="D17" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
@@ -3714,13 +3784,13 @@
         <v>led-bumper-2</v>
       </c>
       <c r="C18" t="s">
-        <v>232</v>
-      </c>
-      <c r="D18" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
@@ -3729,13 +3799,13 @@
         <v>led-bumper-3</v>
       </c>
       <c r="C19" t="s">
-        <v>233</v>
-      </c>
-      <c r="D19" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" s="40" t="s">
         <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
@@ -3744,13 +3814,13 @@
         <v>led-toplane1</v>
       </c>
       <c r="C20" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="40" t="s">
         <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
@@ -3759,13 +3829,13 @@
         <v>led-toplane2</v>
       </c>
       <c r="C21" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="40" t="s">
         <v>95</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
@@ -3774,13 +3844,13 @@
         <v>led-toplane3</v>
       </c>
       <c r="C22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>184</v>
+        <v>191</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>177</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
@@ -3789,13 +3859,13 @@
         <v>led-orbit-t</v>
       </c>
       <c r="C23" t="s">
-        <v>223</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>185</v>
+        <v>216</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>178</v>
       </c>
       <c r="E23" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
@@ -3804,13 +3874,13 @@
         <v>led-target-e1</v>
       </c>
       <c r="C24" t="s">
-        <v>242</v>
-      </c>
-      <c r="D24" s="47" t="s">
-        <v>186</v>
+        <v>235</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
@@ -3819,13 +3889,13 @@
         <v>led-target-e2</v>
       </c>
       <c r="C25" t="s">
-        <v>243</v>
-      </c>
-      <c r="D25" s="47" t="s">
-        <v>187</v>
+        <v>236</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>180</v>
       </c>
       <c r="E25" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
@@ -3834,13 +3904,13 @@
         <v>led-aerial</v>
       </c>
       <c r="C26" t="s">
-        <v>245</v>
-      </c>
-      <c r="D26" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="D26" s="40" t="s">
         <v>96</v>
       </c>
       <c r="E26" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
@@ -3849,13 +3919,13 @@
         <v>led-target-m3</v>
       </c>
       <c r="C27" t="s">
-        <v>262</v>
-      </c>
-      <c r="D27" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="D27" s="40" t="s">
         <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
@@ -3864,13 +3934,13 @@
         <v>led-portal-m</v>
       </c>
       <c r="C28" t="s">
-        <v>247</v>
-      </c>
-      <c r="D28" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" s="40" t="s">
         <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
@@ -3879,13 +3949,13 @@
         <v>led-target-m4</v>
       </c>
       <c r="C29" t="s">
-        <v>261</v>
-      </c>
-      <c r="D29" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="D29" s="40" t="s">
         <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
@@ -3894,13 +3964,13 @@
         <v>led-ramp-l</v>
       </c>
       <c r="C30" t="s">
-        <v>249</v>
-      </c>
-      <c r="D30" s="47" t="s">
-        <v>188</v>
+        <v>242</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>181</v>
       </c>
       <c r="E30" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
@@ -3909,13 +3979,13 @@
         <v>led-orbit-l</v>
       </c>
       <c r="C31" t="s">
-        <v>221</v>
-      </c>
-      <c r="D31" s="47" t="s">
-        <v>189</v>
+        <v>214</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>182</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
@@ -3924,13 +3994,13 @@
         <v>led-button</v>
       </c>
       <c r="C32" t="s">
-        <v>250</v>
-      </c>
-      <c r="D32" s="47" t="s">
-        <v>206</v>
+        <v>243</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>199</v>
       </c>
       <c r="E32" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
@@ -3939,13 +4009,13 @@
         <v>led-target-l1</v>
       </c>
       <c r="C33" t="s">
-        <v>308</v>
-      </c>
-      <c r="D33" s="47" t="s">
-        <v>207</v>
+        <v>301</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
@@ -3954,13 +4024,13 @@
         <v>led-insinerator</v>
       </c>
       <c r="C34" t="s">
-        <v>309</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>234</v>
+        <v>302</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>227</v>
       </c>
       <c r="E34" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
@@ -3969,28 +4039,28 @@
         <v>led-dropper</v>
       </c>
       <c r="C35" t="s">
-        <v>343</v>
-      </c>
-      <c r="D35" s="47" t="s">
-        <v>235</v>
+        <v>335</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>228</v>
       </c>
       <c r="E35" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="42" t="str">
+      <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>led-exit-success</v>
       </c>
-      <c r="C36" s="42" t="s">
-        <v>355</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>236</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>354</v>
+      <c r="C36" t="s">
+        <v>347</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="E36" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
@@ -3998,14 +4068,14 @@
         <f t="shared" si="0"/>
         <v>led-exit-open-1</v>
       </c>
-      <c r="C37" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>237</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>363</v>
+      <c r="C37" t="s">
+        <v>350</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
@@ -4013,14 +4083,14 @@
         <f t="shared" si="0"/>
         <v>led-exit-open-2</v>
       </c>
-      <c r="C38" s="42" t="s">
-        <v>359</v>
-      </c>
-      <c r="D38" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>364</v>
+      <c r="C38" t="s">
+        <v>351</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="E38" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
@@ -4028,14 +4098,14 @@
         <f t="shared" si="0"/>
         <v>led-exit-open-3</v>
       </c>
-      <c r="C39" s="42" t="s">
-        <v>360</v>
-      </c>
-      <c r="D39" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>365</v>
+      <c r="C39" t="s">
+        <v>352</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>232</v>
+      </c>
+      <c r="E39" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
@@ -4043,14 +4113,14 @@
         <f t="shared" si="0"/>
         <v>led-exit-open-4</v>
       </c>
-      <c r="C40" s="42" t="s">
-        <v>361</v>
-      </c>
-      <c r="D40" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>366</v>
+      <c r="C40" t="s">
+        <v>353</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="E40" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
@@ -4058,14 +4128,14 @@
         <f t="shared" si="0"/>
         <v>led-exit-open-5</v>
       </c>
-      <c r="C41" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="D41" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="E41" s="42" t="s">
-        <v>367</v>
+      <c r="C41" t="s">
+        <v>354</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>250</v>
+      </c>
+      <c r="E41" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
@@ -4074,7 +4144,7 @@
         <v>led-</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -4083,7 +4153,7 @@
         <v>led-</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
@@ -4092,7 +4162,7 @@
         <v>led-</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.35">
@@ -4101,7 +4171,7 @@
         <v>led-</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.35">
@@ -4110,7 +4180,7 @@
         <v>led-</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
@@ -4119,7 +4189,7 @@
         <v>led-</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.35">
@@ -4128,7 +4198,7 @@
         <v>led-</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
@@ -4137,7 +4207,7 @@
         <v>led-</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.35">
@@ -4146,7 +4216,7 @@
         <v>led-</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.35">
@@ -4155,7 +4225,7 @@
         <v>led-</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -4198,12 +4268,12 @@
   <sheetData>
     <row r="2" spans="2:105" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="2:105" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="2:105" ht="164.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4601,8 +4671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896D7F36-299A-4BDE-822D-D1A9A709E1EC}">
   <dimension ref="B1:AZ47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="P1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO18" sqref="AO18:AO20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5026,7 +5096,7 @@
     </row>
     <row r="7" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B7" s="33" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C7" s="15" t="str">
         <f>$H$41&amp;"-"&amp;I$32&amp;"-"&amp;E7</f>
@@ -5092,7 +5162,7 @@
       <c r="AL7" s="18"/>
       <c r="AM7" s="18"/>
       <c r="AO7" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="AP7" s="15" t="str">
         <f>$H$41&amp;"-"&amp;AV$32&amp;"-"&amp;AR7</f>
@@ -5117,7 +5187,7 @@
     </row>
     <row r="8" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B8" s="33" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C8" s="15" t="str">
         <f t="shared" ref="C8:C22" si="0">$H$41&amp;"-"&amp;I$32&amp;"-"&amp;E8</f>
@@ -5208,7 +5278,7 @@
       </c>
       <c r="AM8" s="26"/>
       <c r="AO8" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="AP8" s="15" t="str">
         <f t="shared" ref="AP8:AP22" si="3">$H$41&amp;"-"&amp;AV$32&amp;"-"&amp;AR8</f>
@@ -5330,7 +5400,7 @@
       </c>
       <c r="AM9" s="26"/>
       <c r="AO9" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="AP9" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5452,7 +5522,7 @@
       </c>
       <c r="AM10" s="26"/>
       <c r="AO10" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="AP10" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5574,7 +5644,7 @@
       </c>
       <c r="AM11" s="26"/>
       <c r="AO11" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AP11" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5702,7 +5772,7 @@
       </c>
       <c r="AM12" s="26"/>
       <c r="AO12" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="AP12" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5825,8 +5895,8 @@
         <v>2-2-21</v>
       </c>
       <c r="AM13" s="26"/>
-      <c r="AO13" s="42" t="s">
-        <v>316</v>
+      <c r="AO13" t="s">
+        <v>309</v>
       </c>
       <c r="AP13" s="15" t="str">
         <f t="shared" si="3"/>
@@ -5947,6 +6017,9 @@
         <v>2-2-22</v>
       </c>
       <c r="AM14" s="26"/>
+      <c r="AO14" t="s">
+        <v>381</v>
+      </c>
       <c r="AP14" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-7</v>
@@ -5976,7 +6049,7 @@
     </row>
     <row r="15" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B15" s="33" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C15" s="15" t="str">
         <f t="shared" si="0"/>
@@ -6037,7 +6110,7 @@
         <v>2-1-23</v>
       </c>
       <c r="Z15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AC15" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6066,6 +6139,9 @@
         <v>2-2-23</v>
       </c>
       <c r="AM15" s="26"/>
+      <c r="AO15" t="s">
+        <v>382</v>
+      </c>
       <c r="AP15" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-8</v>
@@ -6095,7 +6171,7 @@
     </row>
     <row r="16" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B16" s="33" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C16" s="15" t="str">
         <f t="shared" si="0"/>
@@ -6156,7 +6232,7 @@
         <v>2-1-24</v>
       </c>
       <c r="Z16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AC16" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6185,6 +6261,9 @@
         <v>2-2-24</v>
       </c>
       <c r="AM16" s="26"/>
+      <c r="AO16" t="s">
+        <v>383</v>
+      </c>
       <c r="AP16" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-9</v>
@@ -6214,7 +6293,7 @@
     </row>
     <row r="17" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B17" s="33" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C17" s="15" t="str">
         <f t="shared" si="0"/>
@@ -6275,7 +6354,7 @@
         <v>2-1-25</v>
       </c>
       <c r="Z17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AC17" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6304,6 +6383,9 @@
         <v>2-2-25</v>
       </c>
       <c r="AM17" s="26"/>
+      <c r="AO17" t="s">
+        <v>384</v>
+      </c>
       <c r="AP17" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-10</v>
@@ -6394,7 +6476,7 @@
         <v>2-1-26</v>
       </c>
       <c r="Z18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="AC18" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6423,6 +6505,9 @@
         <v>2-2-26</v>
       </c>
       <c r="AM18" s="26"/>
+      <c r="AO18" s="47" t="s">
+        <v>393</v>
+      </c>
       <c r="AP18" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-11</v>
@@ -6481,7 +6566,7 @@
         <v>2-0-27</v>
       </c>
       <c r="M19" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="O19" s="32" t="s">
         <v>145</v>
@@ -6513,7 +6598,7 @@
         <v>2-1-27</v>
       </c>
       <c r="Z19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AC19" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6542,6 +6627,9 @@
         <v>2-2-27</v>
       </c>
       <c r="AM19" s="26"/>
+      <c r="AO19" s="47" t="s">
+        <v>396</v>
+      </c>
       <c r="AP19" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-12</v>
@@ -6600,7 +6688,7 @@
         <v>2-0-28</v>
       </c>
       <c r="M20" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="O20" s="32" t="s">
         <v>145</v>
@@ -6631,8 +6719,8 @@
         <f t="shared" si="5"/>
         <v>2-1-28</v>
       </c>
-      <c r="Z20" s="34" t="s">
-        <v>173</v>
+      <c r="Z20" s="47" t="s">
+        <v>388</v>
       </c>
       <c r="AC20" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6661,6 +6749,9 @@
         <v>2-2-28</v>
       </c>
       <c r="AM20" s="26"/>
+      <c r="AO20" s="47" t="s">
+        <v>394</v>
+      </c>
       <c r="AP20" s="15" t="str">
         <f t="shared" si="3"/>
         <v>2-3-13</v>
@@ -6718,8 +6809,8 @@
         <f t="shared" si="4"/>
         <v>2-0-29</v>
       </c>
-      <c r="M21" s="34" t="s">
-        <v>165</v>
+      <c r="M21" s="47" t="s">
+        <v>385</v>
       </c>
       <c r="O21" s="32" t="s">
         <v>145</v>
@@ -6750,8 +6841,8 @@
         <f t="shared" si="5"/>
         <v>2-1-29</v>
       </c>
-      <c r="Z21" s="34" t="s">
-        <v>174</v>
+      <c r="Z21" s="47" t="s">
+        <v>391</v>
       </c>
       <c r="AC21" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6809,7 +6900,7 @@
     </row>
     <row r="22" spans="2:52" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C22" s="15" t="str">
         <f t="shared" si="0"/>
@@ -6837,8 +6928,8 @@
         <f t="shared" si="4"/>
         <v>2-0-30</v>
       </c>
-      <c r="M22" s="34" t="s">
-        <v>166</v>
+      <c r="M22" s="47" t="s">
+        <v>386</v>
       </c>
       <c r="O22" s="32" t="s">
         <v>145</v>
@@ -6869,8 +6960,8 @@
         <f t="shared" si="5"/>
         <v>2-1-30</v>
       </c>
-      <c r="Z22" s="34" t="s">
-        <v>175</v>
+      <c r="Z22" s="47" t="s">
+        <v>392</v>
       </c>
       <c r="AC22" s="15" t="str">
         <f t="shared" si="2"/>
@@ -6947,8 +7038,8 @@
         <f t="shared" si="4"/>
         <v>2-0-31</v>
       </c>
-      <c r="M23" s="34" t="s">
-        <v>167</v>
+      <c r="M23" s="47" t="s">
+        <v>387</v>
       </c>
       <c r="O23" s="16"/>
       <c r="P23" s="16"/>
@@ -6970,8 +7061,8 @@
         <f t="shared" si="5"/>
         <v>2-1-31</v>
       </c>
-      <c r="Z23" s="34" t="s">
-        <v>176</v>
+      <c r="Z23" s="47" t="s">
+        <v>395</v>
       </c>
       <c r="AB23" s="16"/>
       <c r="AC23" s="16"/>
@@ -7214,30 +7305,30 @@
     </row>
     <row r="31" spans="2:52" x14ac:dyDescent="0.35">
       <c r="F31" s="3"/>
-      <c r="G31" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="H31" s="36"/>
+      <c r="G31" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="41"/>
       <c r="I31" s="8"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="36" t="str">
+      <c r="T31" s="41" t="str">
         <f>G31</f>
         <v>COM6</v>
       </c>
-      <c r="U31" s="36"/>
+      <c r="U31" s="41"/>
       <c r="V31" s="8"/>
       <c r="AF31" s="3"/>
-      <c r="AG31" s="36" t="str">
+      <c r="AG31" s="41" t="str">
         <f>T31</f>
         <v>COM6</v>
       </c>
-      <c r="AH31" s="36"/>
+      <c r="AH31" s="41"/>
       <c r="AI31" s="8"/>
       <c r="AS31" s="3"/>
-      <c r="AT31" s="36" t="s">
+      <c r="AT31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AU31" s="36"/>
+      <c r="AU31" s="41"/>
       <c r="AV31" s="8"/>
     </row>
     <row r="32" spans="2:52" x14ac:dyDescent="0.35">
@@ -7312,33 +7403,48 @@
       <c r="AU35" s="7"/>
     </row>
     <row r="36" spans="3:48" x14ac:dyDescent="0.35">
-      <c r="G36" s="37" t="s">
+      <c r="G36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H36" s="38"/>
-      <c r="T36" s="37" t="s">
+      <c r="H36" s="43"/>
+      <c r="T36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="U36" s="38"/>
-      <c r="AG36" s="37" t="s">
+      <c r="U36" s="43"/>
+      <c r="Y36" s="47"/>
+      <c r="AG36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="AH36" s="38"/>
-      <c r="AT36" s="37" t="s">
+      <c r="AH36" s="43"/>
+      <c r="AT36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="AU36" s="38"/>
+      <c r="AU36" s="43"/>
     </row>
     <row r="37" spans="3:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G37" s="6"/>
       <c r="H37" s="11"/>
       <c r="T37" s="6"/>
       <c r="U37" s="11"/>
+      <c r="Y37" s="47"/>
       <c r="AG37" s="6"/>
       <c r="AH37" s="11"/>
       <c r="AT37" s="6"/>
       <c r="AU37" s="11"/>
     </row>
+    <row r="38" spans="3:48" x14ac:dyDescent="0.35">
+      <c r="Y38" s="47"/>
+    </row>
+    <row r="39" spans="3:48" x14ac:dyDescent="0.35">
+      <c r="Y39" s="47" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="40" spans="3:48" x14ac:dyDescent="0.35">
+      <c r="Y40" s="47" t="s">
+        <v>396</v>
+      </c>
+    </row>
     <row r="41" spans="3:48" x14ac:dyDescent="0.35">
       <c r="F41" s="25" t="s">
         <v>130</v>
@@ -7347,11 +7453,14 @@
       <c r="H41" s="25">
         <v>2</v>
       </c>
+      <c r="Y41" s="47" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="43" spans="3:48" x14ac:dyDescent="0.35">
       <c r="C43" s="17"/>
       <c r="M43" s="32" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="P43" s="17"/>
       <c r="AC43" s="17"/>
@@ -7366,7 +7475,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="34" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="3:48" x14ac:dyDescent="0.35">
@@ -10067,28 +10176,28 @@
     </row>
     <row r="31" spans="2:44" x14ac:dyDescent="0.35">
       <c r="E31" s="3"/>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="8"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="36" t="s">
+      <c r="Q31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="R31" s="36"/>
+      <c r="R31" s="41"/>
       <c r="S31" s="8"/>
       <c r="AA31" s="3"/>
-      <c r="AB31" s="36" t="s">
+      <c r="AB31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AC31" s="36"/>
+      <c r="AC31" s="41"/>
       <c r="AD31" s="8"/>
       <c r="AL31" s="3"/>
-      <c r="AM31" s="36" t="s">
+      <c r="AM31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="AN31" s="36"/>
+      <c r="AN31" s="41"/>
       <c r="AO31" s="8"/>
     </row>
     <row r="32" spans="2:44" x14ac:dyDescent="0.35">
@@ -10163,22 +10272,22 @@
       <c r="AN35" s="7"/>
     </row>
     <row r="36" spans="2:41" x14ac:dyDescent="0.35">
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="38"/>
-      <c r="Q36" s="37" t="s">
+      <c r="G36" s="43"/>
+      <c r="Q36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="R36" s="38"/>
-      <c r="AB36" s="37" t="s">
+      <c r="R36" s="43"/>
+      <c r="AB36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="AC36" s="38"/>
-      <c r="AM36" s="37" t="s">
+      <c r="AC36" s="43"/>
+      <c r="AM36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="AN36" s="38"/>
+      <c r="AN36" s="43"/>
     </row>
     <row r="37" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F37" s="6"/>
@@ -10392,10 +10501,10 @@
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="44"/>
       <c r="H12" s="8" t="s">
         <v>40</v>
       </c>
@@ -10544,10 +10653,10 @@
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.35">
       <c r="E31" s="3"/>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="36"/>
+      <c r="G31" s="41"/>
       <c r="H31" s="8"/>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.35">
@@ -10569,10 +10678,10 @@
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G36" s="38"/>
+      <c r="G36" s="43"/>
     </row>
     <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F37" s="6"/>

</xml_diff>